<commit_message>
Added trained MLP (neural network) models
</commit_message>
<xml_diff>
--- a/results/12hr_MLP.xlsx
+++ b/results/12hr_MLP.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>bestHyperparameters</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>{'activation': 'relu', 'alpha': 1e-07, 'beta_1': 0.9, 'hidden_layer_sizes': 10, 'learning_rate': 'constant', 'learning_rate_init': 0.01, 'max_iter': 700, 'momentum': 0.9, 'power_t': 0.5, 'random_state': 6, 'solver': 'sgd'}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'alpha': 1e-06, 'beta_1': 0.9, 'hidden_layer_sizes': 10, 'learning_rate': 'constant', 'learning_rate_init': 0.01, 'max_iter': 3000, 'momentum': 0.9, 'power_t': 0.5, 'random_state': 6, 'solver': 'lbfgs'}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'alpha': 1e-06, 'beta_1': 0.9, 'hidden_layer_sizes': 10, 'learning_rate': 'constant', 'learning_rate_init': 0.1, 'max_iter': 500, 'momentum': 0.9, 'power_t': 0.5, 'random_state': 6, 'solver': 'lbfgs'}</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B:B"/>
@@ -622,6 +628,28 @@
         <v>0.8169999999999999</v>
       </c>
     </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.992</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.992</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.783</v>
+      </c>
+    </row>
     <row customHeight="1" ht="13.8" r="1048576" s="4" spans="1:3"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>